<commit_message>
resolve three pdf Tarija
</commit_message>
<xml_diff>
--- a/circulares/CI 02-2/DDE_Tarija.xlsx
+++ b/circulares/CI 02-2/DDE_Tarija.xlsx
@@ -20,7 +20,9 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AFP-NUA'!$A$3:$P$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cert.Nac.!$A$3:$P$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Libreta Mil.'!$A$3:$P$3</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'AFP-NUA'!$A$1:$N$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'AFP-NUA'!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">Cert.Nac.!$1:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Libreta Mil.'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -3900,6 +3902,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3910,15 +3921,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4240,8 +4242,8 @@
   </sheetPr>
   <dimension ref="A1:P153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="P153" sqref="P153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4264,89 +4266,89 @@
     <col min="17" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="11" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="11"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -11856,17 +11858,20 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="K3:L3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -11889,89 +11894,89 @@
     <col min="17" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="11" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="11"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -18581,17 +18586,20 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="K3:L3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.44285714285714284" bottom="0.44285714285714284" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -18615,89 +18623,89 @@
     <col min="17" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+    </row>
+    <row r="3" spans="1:16" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="7" t="s">
+      <c r="L3" s="11"/>
+      <c r="M3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="11" t="s">
+      <c r="N3" s="11"/>
+      <c r="O3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="11"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -31607,7 +31615,7 @@
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="K3:L3"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.31645833333333334" bottom="0.38104166666666667" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="62" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>